<commit_message>
missing samples - arrange by subject, visit
</commit_message>
<xml_diff>
--- a/data/tape_striping_missing_samples.xlsx
+++ b/data/tape_striping_missing_samples.xlsx
@@ -131,6 +131,9 @@
     <t>36</t>
   </si>
   <si>
+    <t>AD_02</t>
+  </si>
+  <si>
     <t>AD_04</t>
   </si>
   <si>
@@ -149,6 +152,9 @@
     <t>AD_09</t>
   </si>
   <si>
+    <t>AD_12</t>
+  </si>
+  <si>
     <t>AD_13</t>
   </si>
   <si>
@@ -158,55 +164,52 @@
     <t>AD_15</t>
   </si>
   <si>
+    <t>AD_16</t>
+  </si>
+  <si>
+    <t>AD_22</t>
+  </si>
+  <si>
+    <t>AD_23</t>
+  </si>
+  <si>
+    <t>AD_25</t>
+  </si>
+  <si>
     <t>AD_30</t>
   </si>
   <si>
+    <t>CO_33</t>
+  </si>
+  <si>
     <t>CO_34</t>
   </si>
   <si>
+    <t>CO_35</t>
+  </si>
+  <si>
+    <t>CO_37</t>
+  </si>
+  <si>
     <t>CO_38</t>
   </si>
   <si>
     <t>CO_39</t>
   </si>
   <si>
-    <t>AD_25</t>
+    <t>CO_42</t>
+  </si>
+  <si>
+    <t>CO_48</t>
+  </si>
+  <si>
+    <t>CO_52</t>
   </si>
   <si>
     <t>CO_56</t>
   </si>
   <si>
-    <t>AD_12</t>
-  </si>
-  <si>
-    <t>CO_52</t>
-  </si>
-  <si>
-    <t>AD_02</t>
-  </si>
-  <si>
-    <t>AD_23</t>
-  </si>
-  <si>
-    <t>CO_48</t>
-  </si>
-  <si>
-    <t>CO_35</t>
-  </si>
-  <si>
-    <t>CO_37</t>
-  </si>
-  <si>
-    <t>AD_16</t>
-  </si>
-  <si>
-    <t>CO_42</t>
-  </si>
-  <si>
-    <t>AD_22</t>
-  </si>
-  <si>
-    <t>CO_33</t>
+    <t>04</t>
   </si>
   <si>
     <t>01</t>
@@ -216,9 +219,6 @@
   </si>
   <si>
     <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
   </si>
   <si>
     <t>05</t>
@@ -299,7 +299,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="n" s="2">
-        <v>43200.0</v>
+        <v>43486.0</v>
       </c>
     </row>
     <row r="3">
@@ -310,7 +310,7 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" t="n" s="2">
         <v>43200.0</v>
@@ -324,10 +324,10 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>43201.0</v>
+        <v>43200.0</v>
       </c>
     </row>
     <row r="5">
@@ -338,10 +338,10 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>43202.0</v>
+        <v>43201.0</v>
       </c>
     </row>
     <row r="6">
@@ -349,13 +349,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>43202.0</v>
+        <v>43298.0</v>
       </c>
     </row>
     <row r="7">
@@ -363,10 +363,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" t="n" s="2">
         <v>43202.0</v>
@@ -377,13 +377,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>43285.0</v>
+        <v>43202.0</v>
       </c>
     </row>
     <row r="9">
@@ -391,13 +391,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>43284.0</v>
+        <v>43202.0</v>
       </c>
     </row>
     <row r="10">
@@ -405,13 +405,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>43277.0</v>
+        <v>43482.0</v>
       </c>
     </row>
     <row r="11">
@@ -419,13 +419,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>43488.0</v>
+        <v>43285.0</v>
       </c>
     </row>
     <row r="12">
@@ -433,13 +433,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>43213.0</v>
+        <v>43486.0</v>
       </c>
     </row>
     <row r="13">
@@ -447,13 +447,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>43237.0</v>
+        <v>43284.0</v>
       </c>
     </row>
     <row r="14">
@@ -461,13 +461,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>43249.0</v>
+        <v>43277.0</v>
       </c>
     </row>
     <row r="15">
@@ -475,13 +475,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" t="n" s="2">
-        <v>43488.0</v>
+        <v>43495.0</v>
       </c>
     </row>
     <row r="16">
@@ -489,13 +489,13 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>43486.0</v>
+        <v>43579.0</v>
       </c>
     </row>
     <row r="17">
@@ -503,13 +503,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>43482.0</v>
+        <v>43766.0</v>
       </c>
     </row>
     <row r="18">
@@ -517,13 +517,13 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>43486.0</v>
+        <v>43476.0</v>
       </c>
     </row>
     <row r="19">
@@ -531,13 +531,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D19" t="n" s="2">
-        <v>43584.0</v>
+        <v>43742.0</v>
       </c>
     </row>
     <row r="20">
@@ -545,13 +545,13 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>43486.0</v>
+        <v>43488.0</v>
       </c>
     </row>
     <row r="21">
@@ -559,13 +559,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D21" t="n" s="2">
-        <v>43742.0</v>
+        <v>43686.0</v>
       </c>
     </row>
     <row r="22">
@@ -573,7 +573,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
@@ -587,13 +587,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" t="n" s="2">
-        <v>43741.0</v>
+        <v>43488.0</v>
       </c>
     </row>
     <row r="24">
@@ -601,13 +601,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D24" t="n" s="2">
-        <v>43214.0</v>
+        <v>43560.0</v>
       </c>
     </row>
     <row r="25">
@@ -615,13 +615,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" t="n" s="2">
-        <v>43229.0</v>
+        <v>43213.0</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>66</v>
       </c>
       <c r="D26" t="n" s="2">
-        <v>43476.0</v>
+        <v>43214.0</v>
       </c>
     </row>
     <row r="27">
@@ -643,13 +643,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" t="n" s="2">
-        <v>43495.0</v>
+        <v>43229.0</v>
       </c>
     </row>
     <row r="28">
@@ -657,13 +657,13 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" t="n" s="2">
-        <v>43686.0</v>
+        <v>43237.0</v>
       </c>
     </row>
     <row r="29">
@@ -671,13 +671,13 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" t="n" s="2">
-        <v>43537.0</v>
+        <v>43249.0</v>
       </c>
     </row>
     <row r="30">
@@ -685,10 +685,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D30" t="n" s="2">
         <v>43537.0</v>
@@ -699,13 +699,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D31" t="n" s="2">
-        <v>43766.0</v>
+        <v>43537.0</v>
       </c>
     </row>
     <row r="32">
@@ -713,7 +713,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>69</v>
@@ -727,13 +727,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D33" t="n" s="2">
-        <v>43727.0</v>
+        <v>43486.0</v>
       </c>
     </row>
     <row r="34">
@@ -741,13 +741,13 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>43298.0</v>
+        <v>43584.0</v>
       </c>
     </row>
     <row r="35">
@@ -755,13 +755,13 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D35" t="n" s="2">
-        <v>43486.0</v>
+        <v>43741.0</v>
       </c>
     </row>
     <row r="36">
@@ -769,13 +769,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" t="n" s="2">
-        <v>43579.0</v>
+        <v>43486.0</v>
       </c>
     </row>
     <row r="37">
@@ -789,7 +789,7 @@
         <v>69</v>
       </c>
       <c r="D37" t="n" s="2">
-        <v>43560.0</v>
+        <v>43727.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>